<commit_message>
funciona para multiples loans
</commit_message>
<xml_diff>
--- a/ScriptPython/clientes.xlsx
+++ b/ScriptPython/clientes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,7 +496,7 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>monthly_payment</t>
+          <t>weekly_payment</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
@@ -536,78 +536,414 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>765</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>JUSTO CORTES DIAZ</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>8990</v>
-      </c>
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
-        <v>600</v>
-      </c>
-      <c r="F2" t="n">
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>8325</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CHARNEQUA BENNET</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>16990</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1440.9</v>
+      </c>
+      <c r="E3" t="n">
+        <v>820</v>
+      </c>
+      <c r="F3" t="n">
         <v>0</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G3" t="n">
+        <v>799</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1185.21</v>
+      </c>
+      <c r="I3" t="n">
+        <v>3000</v>
+      </c>
+      <c r="J3" t="n">
         <v>0</v>
       </c>
-      <c r="H2" t="n">
-        <v>631.34</v>
-      </c>
-      <c r="I2" t="n">
+      <c r="K3" t="n">
+        <v>238</v>
+      </c>
+      <c r="L3" t="n">
+        <v>28.054</v>
+      </c>
+      <c r="M3" t="n">
+        <v>136.23</v>
+      </c>
+      <c r="N3" t="n">
+        <v>7</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>$18,235.11</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>02/24/1983</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>595-20-8868</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>charnequabennet02@gmail.com</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>(772) 301-2514</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>745 North Powerline Road, Pompano Beach FL 33069</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>8326</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CHAD WHYMS</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>11500</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1190.7</v>
+      </c>
+      <c r="E4" t="n">
+        <v>820</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>799</v>
+      </c>
+      <c r="H4" t="n">
+        <v>855.8100000000001</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>208</v>
+      </c>
+      <c r="L4" t="n">
+        <v>28.554</v>
+      </c>
+      <c r="M4" t="n">
+        <v>102.3</v>
+      </c>
+      <c r="N4" t="n">
+        <v>7</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>$12,665.51</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>03/17/1984</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>593-64-4629</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>chadwyms@yahoo.com</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>(786) 617-2472</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>3595 NW 187TH ST, MIAMI GARDENS FL 33056</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>8322</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>JEANNE LUBIN</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>11300</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1128.9</v>
+      </c>
+      <c r="E5" t="n">
+        <v>820</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>799</v>
+      </c>
+      <c r="H5" t="n">
+        <v>843.8100000000001</v>
+      </c>
+      <c r="I5" t="n">
         <v>2000</v>
       </c>
-      <c r="J2" t="n">
+      <c r="J5" t="n">
         <v>0</v>
       </c>
-      <c r="K2" t="n">
-        <v>42</v>
-      </c>
-      <c r="L2" t="n">
-        <v>28</v>
-      </c>
-      <c r="M2" t="n">
-        <v>341.56</v>
-      </c>
-      <c r="N2" t="n">
-        <v>30</v>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>$9,082.19</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>08/06/1947</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>770-24-3815</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>reyluciabrenda@gmail.com</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>(305) 303-2366</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>17221 NW 43 CT, MIAMI FL 33055-4303</t>
+      <c r="K5" t="n">
+        <v>208</v>
+      </c>
+      <c r="L5" t="n">
+        <v>28.556</v>
+      </c>
+      <c r="M5" t="n">
+        <v>104.13</v>
+      </c>
+      <c r="N5" t="n">
+        <v>7</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>$12,891.71</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>01/20/1991</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>766-84-9187</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>jeannelubin1991@gmail.com</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>(786) 805-8896</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>820 Northwest 81st Street, Miami FL 33150</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>8328</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>DIANNY MEDINA</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>11000</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1438.6</v>
+      </c>
+      <c r="E6" t="n">
+        <v>820</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>799</v>
+      </c>
+      <c r="H6" t="n">
+        <v>825.8100000000001</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2200</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>238</v>
+      </c>
+      <c r="L6" t="n">
+        <v>28.05</v>
+      </c>
+      <c r="M6" t="n">
+        <v>94.76000000000001</v>
+      </c>
+      <c r="N6" t="n">
+        <v>7</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>$12,683.41</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>07/30/1970</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>879-30-9526</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>DIANNYMEDINA500@GMAIL.COM</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>(786) 231-7929</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>16720 Northwest 48th Court, Miami Gardens FL 33055</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>8305</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SHAKIERA THOMPSON</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>21990</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1235.7</v>
+      </c>
+      <c r="E7" t="n">
+        <v>820</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>799</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1485.21</v>
+      </c>
+      <c r="I7" t="n">
+        <v>4500</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>238</v>
+      </c>
+      <c r="L7" t="n">
+        <v>28.05</v>
+      </c>
+      <c r="M7" t="n">
+        <v>163.09</v>
+      </c>
+      <c r="N7" t="n">
+        <v>7</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>$21,829.91</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>03/21/1989</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>591-80-0690</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>SHAKIERA21@ICLOUD.COM</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>(229) 343-9706</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>3960 55TH ST NORTH  APT 101, ST PETERSBURG FL 33709</t>
         </is>
       </c>
     </row>

</xml_diff>